<commit_message>
[Carlos Retamales] - Funcionable
</commit_message>
<xml_diff>
--- a/Datos_Oficiales.xlsx
+++ b/Datos_Oficiales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usachcl-my.sharepoint.com/personal/carlos_retamales_a_usach_cl/Documents/2022-2/8°Semestre/MINGESO/MueblesStgo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{87B47BF7-7AAE-4E65-8D3B-417B404E9646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D86DD25-DC42-4865-96D8-FABE4EAB12B9}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{87B47BF7-7AAE-4E65-8D3B-417B404E9646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A702C3D1-F1D1-4D8E-B87E-B5B63E134EA6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E0DAB6D-D2FD-48BF-8EAA-E2D5A880957D}"/>
   </bookViews>
@@ -702,6 +702,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\/mm\/dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,12 +714,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -731,9 +740,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075BBA4D-8325-4071-AB24-23E0E037CE73}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,7 +1096,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1454,7 +1464,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1569,7 +1579,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" t="s">

</xml_diff>